<commit_message>
export daycounter functions to excel (114/1114)
</commit_message>
<xml_diff>
--- a/UnitTests/UnitTests.xlsx
+++ b/UnitTests/UnitTests.xlsx
@@ -10,16 +10,18 @@
     <sheet name="UnitTests" sheetId="1" r:id="rId1"/>
     <sheet name="Calendars" sheetId="2" r:id="rId2"/>
     <sheet name="Date" sheetId="3" r:id="rId3"/>
-    <sheet name="Index" sheetId="4" r:id="rId4"/>
-    <sheet name="TimeSeries" sheetId="5" r:id="rId5"/>
-    <sheet name="Utilities" sheetId="6" r:id="rId6"/>
+    <sheet name="DayCounters" sheetId="4" r:id="rId4"/>
+    <sheet name="Index" sheetId="5" r:id="rId5"/>
+    <sheet name="Quotes" sheetId="6" r:id="rId6"/>
+    <sheet name="TimeSeries" sheetId="7" r:id="rId7"/>
+    <sheet name="Utilities" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="177">
   <si>
     <t>Group</t>
   </si>
@@ -243,6 +245,21 @@
     <t>APR10</t>
   </si>
   <si>
+    <t>DayCounters</t>
+  </si>
+  <si>
+    <t>qlDayCounterName</t>
+  </si>
+  <si>
+    <t>Actual/360</t>
+  </si>
+  <si>
+    <t>qlDayCounterDayCount</t>
+  </si>
+  <si>
+    <t>qlDayCounterYearFraction</t>
+  </si>
+  <si>
     <t>Index</t>
   </si>
   <si>
@@ -294,9 +311,6 @@
     <t>qlInterestRateIndexDayCounter</t>
   </si>
   <si>
-    <t>Actual/360</t>
-  </si>
-  <si>
     <t>qlInterestRateIndexValueDate</t>
   </si>
   <si>
@@ -397,6 +411,105 @@
   </si>
   <si>
     <t>index13#0000</t>
+  </si>
+  <si>
+    <t>Quotes</t>
+  </si>
+  <si>
+    <t>qlQuoteValue</t>
+  </si>
+  <si>
+    <t>qlQuoteIsValid</t>
+  </si>
+  <si>
+    <t>qlSimpleQuoteReset</t>
+  </si>
+  <si>
+    <t>qlSimpleQuoteSetValue</t>
+  </si>
+  <si>
+    <t>qlSimpleQuoteSetTickValue</t>
+  </si>
+  <si>
+    <t>qlSimpleQuoteTickValue</t>
+  </si>
+  <si>
+    <t>qlBucketAnalysis</t>
+  </si>
+  <si>
+    <t>qlBucketAnalysisDelta</t>
+  </si>
+  <si>
+    <t>qlBucketAnalysisDelta2</t>
+  </si>
+  <si>
+    <t>qlSimpleQuote</t>
+  </si>
+  <si>
+    <t>quote01#0000</t>
+  </si>
+  <si>
+    <t>qlForwardValueQuote</t>
+  </si>
+  <si>
+    <t>quote02#0000</t>
+  </si>
+  <si>
+    <t>qlForwardSwapQuote</t>
+  </si>
+  <si>
+    <t>quote03#0000</t>
+  </si>
+  <si>
+    <t>qlImpliedStdDevQuote</t>
+  </si>
+  <si>
+    <t>quote04#0000</t>
+  </si>
+  <si>
+    <t>qlEurodollarFuturesImpliedStdDevQuote</t>
+  </si>
+  <si>
+    <t>quote05#0000</t>
+  </si>
+  <si>
+    <t>qlCompositeQuote</t>
+  </si>
+  <si>
+    <t>quote06#0000</t>
+  </si>
+  <si>
+    <t>qlFuturesConvAdjustmentQuote</t>
+  </si>
+  <si>
+    <t>quote07#0000</t>
+  </si>
+  <si>
+    <t>qlFuturesConvAdjustmentQuoteVolatility</t>
+  </si>
+  <si>
+    <t>qlFuturesConvAdjustmentQuoteMeanReversion</t>
+  </si>
+  <si>
+    <t>qlFuturesConvAdjustmentQuoteImmDate</t>
+  </si>
+  <si>
+    <t>qlFuturesConvAdjustmentQuoteFuturesValue</t>
+  </si>
+  <si>
+    <t>qlLastFixingQuote</t>
+  </si>
+  <si>
+    <t>quote08#0000</t>
+  </si>
+  <si>
+    <t>qlLastFixingQuoteReferenceDate</t>
+  </si>
+  <si>
+    <t>qlRelinkableHandleQuote</t>
+  </si>
+  <si>
+    <t>quote09#0000</t>
   </si>
   <si>
     <t>TimeSeries</t>
@@ -793,7 +906,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -835,12 +948,22 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1866,9 +1989,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1917,7 +2042,7 @@
         <v>76</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f>IF(B3=C3,"PASS","FAIL")</f>
+        <f t="shared" ref="D3:D5" si="0">IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
       <c r="E3" t="s">
@@ -1928,558 +2053,36 @@
       <c r="A4" t="s">
         <v>77</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
+      <c r="B4">
+        <v>364</v>
+      </c>
+      <c r="C4">
+        <v>364</v>
       </c>
       <c r="D4" s="3" t="str">
-        <f t="shared" ref="D4:D34" si="0">IF(B4=C4,"PASS","FAIL")</f>
-        <v>PASS</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E4">
+        <v>364</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>78</v>
       </c>
-      <c r="B5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
+      <c r="B5">
+        <v>1.0111111111111111</v>
+      </c>
+      <c r="C5">
+        <v>1.0111111111111111</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="C6" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="D6" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="E6" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" t="s">
-        <v>91</v>
-      </c>
-      <c r="D14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>92</v>
-      </c>
-      <c r="B15">
-        <v>42709</v>
-      </c>
-      <c r="C15">
-        <v>42709</v>
-      </c>
-      <c r="D15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E15">
-        <v>42709</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16">
-        <v>42703</v>
-      </c>
-      <c r="C16">
-        <v>42703</v>
-      </c>
-      <c r="D16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E16">
-        <v>42703</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B17">
-        <v>43070</v>
-      </c>
-      <c r="C17">
-        <v>43070</v>
-      </c>
-      <c r="D17" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E17">
-        <v>43070</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>95</v>
-      </c>
-      <c r="B18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>97</v>
-      </c>
-      <c r="B19" t="b">
-        <v>1</v>
-      </c>
-      <c r="C19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>98</v>
-      </c>
-      <c r="B20" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E20" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" t="s">
-        <v>101</v>
-      </c>
-      <c r="C21" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E21" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>104</v>
-      </c>
-      <c r="B23" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" t="s">
-        <v>105</v>
-      </c>
-      <c r="D23" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" t="s">
-        <v>107</v>
-      </c>
-      <c r="D24" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E24" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>108</v>
-      </c>
-      <c r="B25" t="s">
-        <v>109</v>
-      </c>
-      <c r="C25" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E25" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>110</v>
-      </c>
-      <c r="B26" t="s">
-        <v>111</v>
-      </c>
-      <c r="C26" t="s">
-        <v>111</v>
-      </c>
-      <c r="D26" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E26" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>112</v>
-      </c>
-      <c r="B27" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E27" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>113</v>
-      </c>
-      <c r="B28" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28" t="s">
-        <v>96</v>
-      </c>
-      <c r="D28" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>114</v>
-      </c>
-      <c r="B29" t="s">
-        <v>115</v>
-      </c>
-      <c r="C29" t="s">
-        <v>115</v>
-      </c>
-      <c r="D29" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E29" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>116</v>
-      </c>
-      <c r="B30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C30" t="s">
-        <v>117</v>
-      </c>
-      <c r="D30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>118</v>
-      </c>
-      <c r="B31" t="s">
-        <v>119</v>
-      </c>
-      <c r="C31" t="s">
-        <v>119</v>
-      </c>
-      <c r="D31" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E31" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>120</v>
-      </c>
-      <c r="B32" t="s">
-        <v>121</v>
-      </c>
-      <c r="C32" t="s">
-        <v>121</v>
-      </c>
-      <c r="D32" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E32" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>122</v>
-      </c>
-      <c r="B33" t="s">
-        <v>123</v>
-      </c>
-      <c r="C33" t="s">
-        <v>123</v>
-      </c>
-      <c r="D33" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E33" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>124</v>
-      </c>
-      <c r="B34" t="s">
-        <v>125</v>
-      </c>
-      <c r="C34" t="s">
-        <v>125</v>
-      </c>
-      <c r="D34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E34" t="s">
-        <v>125</v>
+      <c r="E5">
+        <v>1.0111111111111111</v>
       </c>
     </row>
   </sheetData>
@@ -2488,6 +2091,1067 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:E34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="3" t="str">
+        <f>IF(B3=C3,"PASS","FAIL")</f>
+        <v>PASS</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="str">
+        <f t="shared" ref="D4:D34" si="0">IF(B4=C4,"PASS","FAIL")</f>
+        <v>PASS</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="C6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D6" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E6" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15">
+        <v>42709</v>
+      </c>
+      <c r="C15">
+        <v>42709</v>
+      </c>
+      <c r="D15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E15">
+        <v>42709</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16">
+        <v>42703</v>
+      </c>
+      <c r="C16">
+        <v>42703</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E16">
+        <v>42703</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17">
+        <v>43070</v>
+      </c>
+      <c r="C17">
+        <v>43070</v>
+      </c>
+      <c r="D17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E17">
+        <v>43070</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" t="b">
+        <v>1</v>
+      </c>
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>110</v>
+      </c>
+      <c r="B24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E29" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" t="s">
+        <v>127</v>
+      </c>
+      <c r="D33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>128</v>
+      </c>
+      <c r="B34" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E34" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3">
+        <v>123</v>
+      </c>
+      <c r="C3">
+        <v>123</v>
+      </c>
+      <c r="D3" s="3" t="str">
+        <f>IF(B3=C3,"PASS","FAIL")</f>
+        <v>PASS</v>
+      </c>
+      <c r="E3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="str">
+        <f t="shared" ref="D4:D5" si="0">IF(B4=C4,"PASS","FAIL")</f>
+        <v>PASS</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f>IF(B6=C6,"PASS","FAIL")</f>
+        <v>PASS</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f t="shared" ref="D7:D25" si="1">IF(B7=C7,"PASS","FAIL")</f>
+        <v>PASS</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8">
+        <v>456</v>
+      </c>
+      <c r="C8">
+        <v>456</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="E8">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" t="s">
+        <v>141</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="E12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="E13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="E14" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="E15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="E16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="E17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="E18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19">
+        <v>456</v>
+      </c>
+      <c r="C19">
+        <v>456</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="E19">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20">
+        <v>789</v>
+      </c>
+      <c r="C20">
+        <v>789</v>
+      </c>
+      <c r="D20" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="E20">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>156</v>
+      </c>
+      <c r="B21">
+        <v>43544</v>
+      </c>
+      <c r="C21">
+        <v>43544</v>
+      </c>
+      <c r="D21" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="E21">
+        <v>43544</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B22">
+        <v>123</v>
+      </c>
+      <c r="C22">
+        <v>123</v>
+      </c>
+      <c r="D22" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="E22">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23" t="s">
+        <v>159</v>
+      </c>
+      <c r="C23" t="s">
+        <v>159</v>
+      </c>
+      <c r="D23" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>PASS</v>
+      </c>
+      <c r="E23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>160</v>
+      </c>
+      <c r="B24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="C24" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D24" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E24" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>161</v>
+      </c>
+      <c r="B25" t="s">
+        <v>162</v>
+      </c>
+      <c r="C25" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="D25" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="E25" t="e">
+        <v>#NAME?</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -2533,25 +3197,25 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="D3" s="3" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
       <c r="E3" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="B4">
         <v>25569</v>
@@ -2569,7 +3233,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
       <c r="B5">
         <v>25571</v>
@@ -2587,7 +3251,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>168</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -2605,7 +3269,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>169</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
@@ -2623,7 +3287,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>170</v>
       </c>
       <c r="B8">
         <v>25569</v>
@@ -2641,7 +3305,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>171</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2659,7 +3323,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>135</v>
+        <v>172</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2677,7 +3341,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="B11" t="e">
         <v>#NUM!</v>
@@ -2698,7 +3362,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2744,20 +3408,20 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>176</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>176</v>
       </c>
       <c r="D3" s="3" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
       <c r="E3" t="s">
-        <v>139</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
export schedule functions to excel (200/1114)
</commit_message>
<xml_diff>
--- a/UnitTests/UnitTests.xlsx
+++ b/UnitTests/UnitTests.xlsx
@@ -15,16 +15,17 @@
     <sheet name="PiecewiseYieldCurve" sheetId="6" r:id="rId6"/>
     <sheet name="Quotes" sheetId="7" r:id="rId7"/>
     <sheet name="RateHelpers" sheetId="8" r:id="rId8"/>
-    <sheet name="TermStructures" sheetId="9" r:id="rId9"/>
-    <sheet name="TimeSeries" sheetId="10" r:id="rId10"/>
-    <sheet name="Utilities" sheetId="11" r:id="rId11"/>
+    <sheet name="Schedules" sheetId="9" r:id="rId9"/>
+    <sheet name="TermStructures" sheetId="10" r:id="rId10"/>
+    <sheet name="TimeSeries" sheetId="11" r:id="rId11"/>
+    <sheet name="Utilities" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="294">
   <si>
     <t>Group</t>
   </si>
@@ -695,10 +696,76 @@
     <t>obj_0000e</t>
   </si>
   <si>
-    <t>obj_0002b</t>
+    <t>obj_0002e</t>
   </si>
   <si>
     <t>qlRateHelperRate</t>
+  </si>
+  <si>
+    <t>Schedules</t>
+  </si>
+  <si>
+    <t>qlScheduleSize</t>
+  </si>
+  <si>
+    <t>qlSchedulePreviousDate</t>
+  </si>
+  <si>
+    <t>qlScheduleNextDate</t>
+  </si>
+  <si>
+    <t>qlScheduleDates</t>
+  </si>
+  <si>
+    <t>qlScheduleIsRegular</t>
+  </si>
+  <si>
+    <t>qlScheduleEmpty</t>
+  </si>
+  <si>
+    <t>qlScheduleCalendar</t>
+  </si>
+  <si>
+    <t>qlScheduleStartDate</t>
+  </si>
+  <si>
+    <t>qlScheduleEndDate</t>
+  </si>
+  <si>
+    <t>qlScheduleTenor</t>
+  </si>
+  <si>
+    <t>qlScheduleBDC</t>
+  </si>
+  <si>
+    <t>qlScheduleTerminationDateBDC</t>
+  </si>
+  <si>
+    <t>qlScheduleRule</t>
+  </si>
+  <si>
+    <t>Backward</t>
+  </si>
+  <si>
+    <t>qlScheduleEndOfMonth</t>
+  </si>
+  <si>
+    <t>qlSchedule</t>
+  </si>
+  <si>
+    <t>sched01#0000</t>
+  </si>
+  <si>
+    <t>qlScheduleFromDateVector</t>
+  </si>
+  <si>
+    <t>sched02#0000</t>
+  </si>
+  <si>
+    <t>qlScheduleTruncated</t>
+  </si>
+  <si>
+    <t>sched03#0000</t>
   </si>
   <si>
     <t>TermStructures</t>
@@ -883,7 +950,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -894,6 +961,7 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1195,7 +1263,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1262,12 +1330,17 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>269</v>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -1276,6 +1349,469 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D3" s="3" t="str">
+        <f t="shared" ref="D3:D25" si="0">IF(B3=C3,"PASS","FAIL")</f>
+        <v>PASS</v>
+      </c>
+      <c r="E3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B4">
+        <v>42738</v>
+      </c>
+      <c r="C4">
+        <v>42738</v>
+      </c>
+      <c r="D4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E4">
+        <v>42738</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B5">
+        <v>42736</v>
+      </c>
+      <c r="C5">
+        <v>42736</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E5">
+        <v>42736</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>255</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B10">
+        <v>-180</v>
+      </c>
+      <c r="C10">
+        <v>-180</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E10">
+        <v>-180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>257</v>
+      </c>
+      <c r="B11">
+        <v>-180</v>
+      </c>
+      <c r="C11" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="D11" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="E11" t="e">
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12">
+        <v>-252.99872090438052</v>
+      </c>
+      <c r="C12">
+        <v>-252.99872090438052</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E12">
+        <v>-252.99872090438052</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>259</v>
+      </c>
+      <c r="B13" t="s">
+        <v>260</v>
+      </c>
+      <c r="C13" t="s">
+        <v>260</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E13" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>261</v>
+      </c>
+      <c r="B14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C14" t="s">
+        <v>262</v>
+      </c>
+      <c r="D14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E14" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>263</v>
+      </c>
+      <c r="B15" t="s">
+        <v>264</v>
+      </c>
+      <c r="C15" t="s">
+        <v>264</v>
+      </c>
+      <c r="D15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E15" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>265</v>
+      </c>
+      <c r="B16" t="s">
+        <v>266</v>
+      </c>
+      <c r="C16" t="s">
+        <v>266</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E16" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>267</v>
+      </c>
+      <c r="B17" t="s">
+        <v>268</v>
+      </c>
+      <c r="C17" t="s">
+        <v>268</v>
+      </c>
+      <c r="D17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E17" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>269</v>
+      </c>
+      <c r="B18" t="s">
+        <v>270</v>
+      </c>
+      <c r="C18" t="s">
+        <v>270</v>
+      </c>
+      <c r="D18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E18" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>271</v>
+      </c>
+      <c r="B19" t="s">
+        <v>272</v>
+      </c>
+      <c r="C19" t="s">
+        <v>272</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E19" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>273</v>
+      </c>
+      <c r="B20" t="s">
+        <v>274</v>
+      </c>
+      <c r="C20" t="s">
+        <v>274</v>
+      </c>
+      <c r="D20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E20" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>275</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>276</v>
+      </c>
+      <c r="B22">
+        <v>42736</v>
+      </c>
+      <c r="C22">
+        <v>42736</v>
+      </c>
+      <c r="D22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E22">
+        <v>42736</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>277</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>278</v>
+      </c>
+      <c r="B24">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="C24">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="D24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E24">
+        <v>8.3333333333333332E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>279</v>
+      </c>
+      <c r="B25">
+        <v>42739</v>
+      </c>
+      <c r="C25">
+        <v>42739</v>
+      </c>
+      <c r="D25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E25">
+        <v>42739</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -1321,25 +1857,25 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>259</v>
+        <v>281</v>
       </c>
       <c r="B3" t="s">
-        <v>260</v>
+        <v>282</v>
       </c>
       <c r="C3" t="s">
-        <v>260</v>
+        <v>282</v>
       </c>
       <c r="D3" s="3" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
       <c r="E3" t="s">
-        <v>260</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>261</v>
+        <v>283</v>
       </c>
       <c r="B4">
         <v>25569</v>
@@ -1357,7 +1893,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>262</v>
+        <v>284</v>
       </c>
       <c r="B5">
         <v>25571</v>
@@ -1375,7 +1911,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>263</v>
+        <v>285</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -1393,7 +1929,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>264</v>
+        <v>286</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
@@ -1411,7 +1947,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>265</v>
+        <v>287</v>
       </c>
       <c r="B8">
         <v>25569</v>
@@ -1429,7 +1965,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>266</v>
+        <v>288</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1447,7 +1983,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>267</v>
+        <v>289</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1465,7 +2001,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>268</v>
+        <v>290</v>
       </c>
       <c r="B11" t="e">
         <v>#NUM!</v>
@@ -1486,7 +2022,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -1532,20 +2068,20 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>270</v>
+        <v>292</v>
       </c>
       <c r="B3" t="s">
-        <v>271</v>
+        <v>293</v>
       </c>
       <c r="C3" t="s">
-        <v>271</v>
+        <v>293</v>
       </c>
       <c r="D3" s="3" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
       <c r="E3" t="s">
-        <v>271</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -2338,14 +2874,14 @@
         <v>38371</v>
       </c>
       <c r="C30">
-        <v>25569</v>
+        <v>38371</v>
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E30">
-        <v>25569</v>
+        <v>38371</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3301,7 +3837,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3401,14 +3939,14 @@
         <v>42676</v>
       </c>
       <c r="C6" s="5">
-        <v>42676</v>
+        <v>42677</v>
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
+        <v>FAIL</v>
       </c>
       <c r="E6" s="5">
-        <v>42676</v>
+        <v>42677</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3437,14 +3975,14 @@
         <v>-47.519444444444446</v>
       </c>
       <c r="C8">
-        <v>-47.519444444444446</v>
+        <v>-47.522222222222226</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
+        <v>FAIL</v>
       </c>
       <c r="E8">
-        <v>-47.519444444444446</v>
+        <v>-47.522222222222226</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3958,14 +4496,14 @@
         <v>42678</v>
       </c>
       <c r="C3">
-        <v>42678</v>
+        <v>42681</v>
       </c>
       <c r="D3" s="3" t="str">
         <f t="shared" ref="D3:D35" si="0">IF(B3=C3,"PASS","FAIL")</f>
-        <v>PASS</v>
+        <v>FAIL</v>
       </c>
       <c r="E3">
-        <v>42678</v>
+        <v>42681</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3976,14 +4514,14 @@
         <v>42681</v>
       </c>
       <c r="C4">
-        <v>42681</v>
+        <v>42682</v>
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
+        <v>FAIL</v>
       </c>
       <c r="E4">
-        <v>42681</v>
+        <v>42682</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3994,14 +4532,14 @@
         <v>42681</v>
       </c>
       <c r="C5">
-        <v>42681</v>
+        <v>42682</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
+        <v>FAIL</v>
       </c>
       <c r="E5">
-        <v>42681</v>
+        <v>42682</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -4012,14 +4550,14 @@
         <v>42681</v>
       </c>
       <c r="C6" s="5">
-        <v>42681</v>
+        <v>42682</v>
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
+        <v>FAIL</v>
       </c>
       <c r="E6" s="5">
-        <v>42681</v>
+        <v>42682</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -4545,11 +5083,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:E25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4591,414 +5127,306 @@
       <c r="A3" t="s">
         <v>226</v>
       </c>
-      <c r="B3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C3" t="s">
-        <v>227</v>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f t="shared" ref="D3:D25" si="0">IF(B3=C3,"PASS","FAIL")</f>
-        <v>PASS</v>
-      </c>
-      <c r="E3" t="s">
-        <v>227</v>
+        <f t="shared" ref="D3:D19" si="0">IF(B3=C3,"PASS","FAIL")</f>
+        <v>PASS</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>228</v>
-      </c>
-      <c r="B4">
-        <v>42738</v>
-      </c>
-      <c r="C4">
-        <v>42738</v>
+        <v>227</v>
+      </c>
+      <c r="B4" s="5">
+        <v>25573</v>
+      </c>
+      <c r="C4" s="6">
+        <v>25573</v>
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="E4">
-        <v>42738</v>
+      <c r="E4" s="5">
+        <v>25573</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B5">
-        <v>42736</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>42736</v>
+        <v>0</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
       <c r="E5">
-        <v>42736</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>230</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
+        <v>229</v>
+      </c>
+      <c r="B6" s="5">
+        <v>25570</v>
+      </c>
+      <c r="C6" s="5">
+        <v>25570</v>
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="E6">
-        <v>0</v>
+      <c r="E6" s="5">
+        <v>25570</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>231</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
+        <v>230</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
       </c>
       <c r="D7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="E7" t="s">
-        <v>14</v>
+      <c r="E7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>232</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
+        <v>231</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" t="b">
         <v>0</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>233</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
+        <v>232</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="E9">
-        <v>1</v>
+      <c r="E9" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>234</v>
-      </c>
-      <c r="B10">
-        <v>-180</v>
-      </c>
-      <c r="C10">
-        <v>-180</v>
+        <v>233</v>
+      </c>
+      <c r="B10" s="5">
+        <v>25570</v>
+      </c>
+      <c r="C10" s="6">
+        <v>25570</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="E10">
-        <v>-180</v>
+      <c r="E10" s="5">
+        <v>25570</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>235</v>
-      </c>
-      <c r="B11">
-        <v>-180</v>
-      </c>
-      <c r="C11" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="D11" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="E11" t="e">
-        <v>#NAME?</v>
+        <v>234</v>
+      </c>
+      <c r="B11" s="5">
+        <v>25573</v>
+      </c>
+      <c r="C11" s="6">
+        <v>25573</v>
+      </c>
+      <c r="D11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E11" s="5">
+        <v>25573</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>236</v>
-      </c>
-      <c r="B12">
-        <v>-252.99872090438052</v>
-      </c>
-      <c r="C12">
-        <v>-252.99872090438052</v>
+        <v>235</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
-      <c r="E12">
-        <v>-252.99872090438052</v>
+      <c r="E12" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B13" t="s">
-        <v>238</v>
+        <v>100</v>
       </c>
       <c r="C13" t="s">
-        <v>238</v>
+        <v>100</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
       <c r="E13" t="s">
-        <v>238</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B14" t="s">
-        <v>240</v>
+        <v>100</v>
       </c>
       <c r="C14" t="s">
-        <v>240</v>
+        <v>100</v>
       </c>
       <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
       <c r="E14" t="s">
-        <v>240</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B15" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C15" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
       <c r="E15" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>243</v>
-      </c>
-      <c r="B16" t="s">
-        <v>244</v>
-      </c>
-      <c r="C16" t="s">
-        <v>244</v>
+        <v>240</v>
+      </c>
+      <c r="B16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" t="b">
+        <v>1</v>
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E16" t="s">
-        <v>244</v>
+        <v>FAIL</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B17" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C17" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
       <c r="E17" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B18" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C18" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
       <c r="E18" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B19" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C19" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" si="0"/>
         <v>PASS</v>
       </c>
       <c r="E19" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>251</v>
-      </c>
-      <c r="B20" t="s">
-        <v>252</v>
-      </c>
-      <c r="C20" t="s">
-        <v>252</v>
-      </c>
-      <c r="D20" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E20" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>253</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>254</v>
-      </c>
-      <c r="B22">
-        <v>42736</v>
-      </c>
-      <c r="C22">
-        <v>42736</v>
-      </c>
-      <c r="D22" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E22">
-        <v>42736</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>255</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>256</v>
-      </c>
-      <c r="B24">
-        <v>8.3333333333333332E-3</v>
-      </c>
-      <c r="C24">
-        <v>8.3333333333333332E-3</v>
-      </c>
-      <c r="D24" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E24">
-        <v>8.3333333333333332E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>257</v>
-      </c>
-      <c r="B25">
-        <v>42739</v>
-      </c>
-      <c r="C25">
-        <v>42739</v>
-      </c>
-      <c r="D25" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>PASS</v>
-      </c>
-      <c r="E25">
-        <v>42739</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
export all prices functions to Excel (691/1114)
</commit_message>
<xml_diff>
--- a/UnitTests/UnitTests.xlsx
+++ b/UnitTests/UnitTests.xlsx
@@ -29,20 +29,21 @@
     <sheet name="Optimization" sheetId="20" r:id="rId20"/>
     <sheet name="Payoffs" sheetId="21" r:id="rId21"/>
     <sheet name="PiecewiseYieldCurve" sheetId="22" r:id="rId22"/>
-    <sheet name="PricingEngines" sheetId="23" r:id="rId23"/>
-    <sheet name="Processes" sheetId="24" r:id="rId24"/>
-    <sheet name="Quotes" sheetId="25" r:id="rId25"/>
-    <sheet name="RateHelpers" sheetId="26" r:id="rId26"/>
-    <sheet name="Schedules" sheetId="27" r:id="rId27"/>
-    <sheet name="ShortRateModels" sheetId="28" r:id="rId28"/>
-    <sheet name="SmileSection" sheetId="29" r:id="rId29"/>
-    <sheet name="Swap" sheetId="30" r:id="rId30"/>
-    <sheet name="SwaptionVolatility" sheetId="31" r:id="rId31"/>
-    <sheet name="TermStructures" sheetId="32" r:id="rId32"/>
-    <sheet name="TimeSeries" sheetId="33" r:id="rId33"/>
-    <sheet name="Utilities" sheetId="34" r:id="rId34"/>
-    <sheet name="VanillaSwap" sheetId="35" r:id="rId35"/>
-    <sheet name="Volatilities" sheetId="36" r:id="rId36"/>
+    <sheet name="Prices" sheetId="23" r:id="rId23"/>
+    <sheet name="PricingEngines" sheetId="24" r:id="rId24"/>
+    <sheet name="Processes" sheetId="25" r:id="rId25"/>
+    <sheet name="Quotes" sheetId="26" r:id="rId26"/>
+    <sheet name="RateHelpers" sheetId="27" r:id="rId27"/>
+    <sheet name="Schedules" sheetId="28" r:id="rId28"/>
+    <sheet name="ShortRateModels" sheetId="29" r:id="rId29"/>
+    <sheet name="SmileSection" sheetId="30" r:id="rId30"/>
+    <sheet name="Swap" sheetId="31" r:id="rId31"/>
+    <sheet name="SwaptionVolatility" sheetId="32" r:id="rId32"/>
+    <sheet name="TermStructures" sheetId="33" r:id="rId33"/>
+    <sheet name="TimeSeries" sheetId="34" r:id="rId34"/>
+    <sheet name="Utilities" sheetId="35" r:id="rId35"/>
+    <sheet name="VanillaSwap" sheetId="36" r:id="rId36"/>
+    <sheet name="Volatilities" sheetId="37" r:id="rId37"/>
   </sheets>
   <definedNames>
     <definedName name="UNIT_TEST" localSheetId="1">AssetSwap!$A$3:$E$12</definedName>
@@ -66,27 +67,28 @@
     <definedName name="UNIT_TEST" localSheetId="19">Optimization!$A$3:$E$15</definedName>
     <definedName name="UNIT_TEST" localSheetId="20">Payoffs!$A$3:$E$16</definedName>
     <definedName name="UNIT_TEST" localSheetId="21">PiecewiseYieldCurve!$A$3:$E$9</definedName>
-    <definedName name="UNIT_TEST" localSheetId="22">PricingEngines!$A$3:$E$55</definedName>
-    <definedName name="UNIT_TEST" localSheetId="23">Processes!$A$3:$E$3</definedName>
-    <definedName name="UNIT_TEST" localSheetId="24">Quotes!$A$3:$E$25</definedName>
-    <definedName name="UNIT_TEST" localSheetId="25">RateHelpers!$A$3:$E$35</definedName>
-    <definedName name="UNIT_TEST" localSheetId="26">Schedules!$A$3:$E$19</definedName>
-    <definedName name="UNIT_TEST" localSheetId="27">ShortRateModels!$A$3:$E$15</definedName>
-    <definedName name="UNIT_TEST" localSheetId="28">SmileSection!$A$3:$E$20</definedName>
-    <definedName name="UNIT_TEST" localSheetId="29">Swap!$A$3:$E$9</definedName>
-    <definedName name="UNIT_TEST" localSheetId="30">SwaptionVolatility!$A$3:$E$29</definedName>
-    <definedName name="UNIT_TEST" localSheetId="31">TermStructures!$A$3:$E$25</definedName>
-    <definedName name="UNIT_TEST" localSheetId="32">TimeSeries!$A$3:$E$11</definedName>
-    <definedName name="UNIT_TEST" localSheetId="33">Utilities!$A$3:$E$3</definedName>
-    <definedName name="UNIT_TEST" localSheetId="34">VanillaSwap!$A$3:$E$22</definedName>
-    <definedName name="UNIT_TEST" localSheetId="35">Volatilities!$A$3:$E$36</definedName>
+    <definedName name="UNIT_TEST" localSheetId="22">Prices!$A$3:$E$4</definedName>
+    <definedName name="UNIT_TEST" localSheetId="23">PricingEngines!$A$3:$E$55</definedName>
+    <definedName name="UNIT_TEST" localSheetId="24">Processes!$A$3:$E$3</definedName>
+    <definedName name="UNIT_TEST" localSheetId="25">Quotes!$A$3:$E$25</definedName>
+    <definedName name="UNIT_TEST" localSheetId="26">RateHelpers!$A$3:$E$35</definedName>
+    <definedName name="UNIT_TEST" localSheetId="27">Schedules!$A$3:$E$19</definedName>
+    <definedName name="UNIT_TEST" localSheetId="28">ShortRateModels!$A$3:$E$15</definedName>
+    <definedName name="UNIT_TEST" localSheetId="29">SmileSection!$A$3:$E$20</definedName>
+    <definedName name="UNIT_TEST" localSheetId="30">Swap!$A$3:$E$9</definedName>
+    <definedName name="UNIT_TEST" localSheetId="31">SwaptionVolatility!$A$3:$E$29</definedName>
+    <definedName name="UNIT_TEST" localSheetId="32">TermStructures!$A$3:$E$25</definedName>
+    <definedName name="UNIT_TEST" localSheetId="33">TimeSeries!$A$3:$E$11</definedName>
+    <definedName name="UNIT_TEST" localSheetId="34">Utilities!$A$3:$E$3</definedName>
+    <definedName name="UNIT_TEST" localSheetId="35">VanillaSwap!$A$3:$E$22</definedName>
+    <definedName name="UNIT_TEST" localSheetId="36">Volatilities!$A$3:$E$36</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2459" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2474" uniqueCount="938">
   <si>
     <t>Group</t>
   </si>
@@ -1762,6 +1764,15 @@
     <t>PiecewiseYieldCurve</t>
   </si>
   <si>
+    <t>qlMidEquivalent</t>
+  </si>
+  <si>
+    <t>qlMidSafe</t>
+  </si>
+  <si>
+    <t>Prices</t>
+  </si>
+  <si>
     <t>qlBlackFormula</t>
   </si>
   <si>
@@ -2230,7 +2241,7 @@
     <t>obj_000a0</t>
   </si>
   <si>
-    <t>obj_000d5</t>
+    <t>obj_000d6</t>
   </si>
   <si>
     <t>qlRateHelperRate</t>
@@ -3250,7 +3261,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3806,23 +3817,23 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>629</v>
+        <v>560</v>
       </c>
       <c r="B23">
-        <f>COUNTIF(PricingEngines!D3:D55,"ERROR")</f>
-        <v>6</v>
+        <f>COUNTIF(Prices!D3:D4,"ERROR")</f>
+        <v>0</v>
       </c>
       <c r="C23">
-        <f>COUNTIF(PricingEngines!D3:D55,"FAIL")</f>
+        <f>COUNTIF(Prices!D3:D4,"FAIL")</f>
         <v>0</v>
       </c>
       <c r="D23">
-        <f>COUNTIF(PricingEngines!D3:D55,"PASS")</f>
-        <v>47</v>
+        <f>COUNTIF(Prices!D3:D4,"PASS")</f>
+        <v>2</v>
       </c>
       <c r="E23">
         <f>SUM(C23:D23)</f>
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="F23" s="7">
         <f>D23/E23</f>
@@ -3834,20 +3845,20 @@
         <v>632</v>
       </c>
       <c r="B24">
-        <f>COUNTIF(Processes!D3,"ERROR")</f>
-        <v>0</v>
+        <f>COUNTIF(PricingEngines!D3:D55,"ERROR")</f>
+        <v>6</v>
       </c>
       <c r="C24">
-        <f>COUNTIF(Processes!D3,"FAIL")</f>
+        <f>COUNTIF(PricingEngines!D3:D55,"FAIL")</f>
         <v>0</v>
       </c>
       <c r="D24">
-        <f>COUNTIF(Processes!D3,"PASS")</f>
-        <v>1</v>
+        <f>COUNTIF(PricingEngines!D3:D55,"PASS")</f>
+        <v>47</v>
       </c>
       <c r="E24">
         <f>SUM(C24:D24)</f>
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="F24" s="7">
         <f>D24/E24</f>
@@ -3856,327 +3867,352 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>665</v>
+        <v>635</v>
       </c>
       <c r="B25">
+        <f>COUNTIF(Processes!D3,"ERROR")</f>
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <f>COUNTIF(Processes!D3,"FAIL")</f>
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <f>COUNTIF(Processes!D3,"PASS")</f>
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <f>SUM(C25:D25)</f>
+        <v>1</v>
+      </c>
+      <c r="F25" s="7">
+        <f>D25/E25</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>668</v>
+      </c>
+      <c r="B26">
         <f>COUNTIF(Quotes!D3:D25,"ERROR")</f>
         <v>0</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <f>COUNTIF(Quotes!D3:D25,"FAIL")</f>
         <v>1</v>
       </c>
-      <c r="D25">
+      <c r="D26">
         <f>COUNTIF(Quotes!D3:D25,"PASS")</f>
         <v>22</v>
       </c>
-      <c r="E25">
-        <f>SUM(C25:D25)</f>
+      <c r="E26">
+        <f>SUM(C26:D26)</f>
         <v>23</v>
       </c>
-      <c r="F25" s="7">
-        <f>D25/E25</f>
+      <c r="F26" s="7">
+        <f>D26/E26</f>
         <v>0.95652173913043481</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>716</v>
-      </c>
-      <c r="B26">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>719</v>
+      </c>
+      <c r="B27">
         <f>COUNTIF(RateHelpers!D3:D35,"ERROR")</f>
         <v>2</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <f>COUNTIF(RateHelpers!D3:D35,"FAIL")</f>
         <v>4</v>
       </c>
-      <c r="D26">
+      <c r="D27">
         <f>COUNTIF(RateHelpers!D3:D35,"PASS")</f>
         <v>27</v>
       </c>
-      <c r="E26">
-        <f>SUM(C26:D26)</f>
-        <v>31</v>
-      </c>
-      <c r="F26" s="7">
-        <f>D26/E26</f>
-        <v>0.87096774193548387</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>738</v>
-      </c>
-      <c r="B27">
-        <f>COUNTIF(Schedules!D3:D19,"ERROR")</f>
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <f>COUNTIF(Schedules!D3:D19,"FAIL")</f>
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <f>COUNTIF(Schedules!D3:D19,"PASS")</f>
-        <v>16</v>
-      </c>
       <c r="E27">
         <f>SUM(C27:D27)</f>
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="F27" s="7">
         <f>D27/E27</f>
-        <v>0.94117647058823528</v>
+        <v>0.87096774193548387</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>755</v>
+        <v>741</v>
       </c>
       <c r="B28">
+        <f>COUNTIF(Schedules!D3:D19,"ERROR")</f>
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <f>COUNTIF(Schedules!D3:D19,"FAIL")</f>
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <f>COUNTIF(Schedules!D3:D19,"PASS")</f>
+        <v>17</v>
+      </c>
+      <c r="E28">
+        <f>SUM(C28:D28)</f>
+        <v>17</v>
+      </c>
+      <c r="F28" s="7">
+        <f>D28/E28</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>758</v>
+      </c>
+      <c r="B29">
         <f>COUNTIF(ShortRateModels!D3:D15,"ERROR")</f>
         <v>0</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <f>COUNTIF(ShortRateModels!D3:D15,"FAIL")</f>
         <v>0</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <f>COUNTIF(ShortRateModels!D3:D15,"PASS")</f>
         <v>13</v>
       </c>
-      <c r="E28">
-        <f>SUM(C28:D28)</f>
+      <c r="E29">
+        <f>SUM(C29:D29)</f>
         <v>13</v>
       </c>
-      <c r="F28" s="7">
-        <f>D28/E28</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>778</v>
-      </c>
-      <c r="B29">
+      <c r="F29" s="7">
+        <f>D29/E29</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>781</v>
+      </c>
+      <c r="B30">
         <f>COUNTIF(SmileSection!D3:D20,"ERROR")</f>
         <v>9</v>
       </c>
-      <c r="C29">
+      <c r="C30">
         <f>COUNTIF(SmileSection!D3:D20,"FAIL")</f>
         <v>0</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <f>COUNTIF(SmileSection!D3:D20,"PASS")</f>
         <v>9</v>
       </c>
-      <c r="E29">
-        <f>SUM(C29:D29)</f>
+      <c r="E30">
+        <f>SUM(C30:D30)</f>
         <v>9</v>
       </c>
-      <c r="F29" s="7">
-        <f>D29/E29</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>788</v>
-      </c>
-      <c r="B30">
+      <c r="F30" s="7">
+        <f>D30/E30</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>791</v>
+      </c>
+      <c r="B31">
         <f>COUNTIF(Swap!D3:D9,"ERROR")</f>
         <v>0</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <f>COUNTIF(Swap!D3:D9,"FAIL")</f>
         <v>1</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <f>COUNTIF(Swap!D3:D9,"PASS")</f>
         <v>6</v>
       </c>
-      <c r="E30">
-        <f>SUM(C30:D30)</f>
+      <c r="E31">
+        <f>SUM(C31:D31)</f>
         <v>7</v>
       </c>
-      <c r="F30" s="7">
-        <f>D30/E30</f>
+      <c r="F31" s="7">
+        <f>D31/E31</f>
         <v>0.8571428571428571</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>820</v>
-      </c>
-      <c r="B31">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>823</v>
+      </c>
+      <c r="B32">
         <f>COUNTIF(SwaptionVolatility!D3:D29,"ERROR")</f>
         <v>15</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <f>COUNTIF(SwaptionVolatility!D3:D29,"FAIL")</f>
         <v>0</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <f>COUNTIF(SwaptionVolatility!D3:D29,"PASS")</f>
         <v>12</v>
       </c>
-      <c r="E31">
-        <f>SUM(C31:D31)</f>
+      <c r="E32">
+        <f>SUM(C32:D32)</f>
         <v>12</v>
       </c>
-      <c r="F31" s="7">
-        <f>D31/E31</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>853</v>
-      </c>
-      <c r="B32">
+      <c r="F32" s="7">
+        <f>D32/E32</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>856</v>
+      </c>
+      <c r="B33">
         <f>COUNTIF(TermStructures!D3:D25,"ERROR")</f>
         <v>0</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <f>COUNTIF(TermStructures!D3:D25,"FAIL")</f>
         <v>0</v>
       </c>
-      <c r="D32">
+      <c r="D33">
         <f>COUNTIF(TermStructures!D3:D25,"PASS")</f>
         <v>23</v>
       </c>
-      <c r="E32">
-        <f>SUM(C32:D32)</f>
+      <c r="E33">
+        <f>SUM(C33:D33)</f>
         <v>23</v>
       </c>
-      <c r="F32" s="7">
-        <f>D32/E32</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>864</v>
-      </c>
-      <c r="B33">
+      <c r="F33" s="7">
+        <f>D33/E33</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>867</v>
+      </c>
+      <c r="B34">
         <f>COUNTIF(TimeSeries!D3:D11,"ERROR")</f>
         <v>1</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <f>COUNTIF(TimeSeries!D3:D11,"FAIL")</f>
         <v>0</v>
       </c>
-      <c r="D33">
+      <c r="D34">
         <f>COUNTIF(TimeSeries!D3:D11,"PASS")</f>
         <v>8</v>
       </c>
-      <c r="E33">
-        <f>SUM(C33:D33)</f>
-        <v>8</v>
-      </c>
-      <c r="F33" s="7">
-        <f>D33/E33</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>868</v>
-      </c>
-      <c r="B34">
-        <f>COUNTIF(Utilities!D3,"ERROR")</f>
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <f>COUNTIF(Utilities!D3,"FAIL")</f>
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <f>COUNTIF(Utilities!D3,"PASS")</f>
-        <v>0</v>
-      </c>
       <c r="E34">
         <f>SUM(C34:D34)</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F34" s="7">
         <f>D34/E34</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>897</v>
+        <v>871</v>
       </c>
       <c r="B35">
+        <f>COUNTIF(Utilities!D3,"ERROR")</f>
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <f>COUNTIF(Utilities!D3,"FAIL")</f>
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <f>COUNTIF(Utilities!D3,"PASS")</f>
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <f>SUM(C35:D35)</f>
+        <v>1</v>
+      </c>
+      <c r="F35" s="7">
+        <f>D35/E35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>900</v>
+      </c>
+      <c r="B36">
         <f>COUNTIF(VanillaSwap!D3:D22,"ERROR")</f>
         <v>0</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <f>COUNTIF(VanillaSwap!D3:D22,"FAIL")</f>
         <v>0</v>
       </c>
-      <c r="D35">
+      <c r="D36">
         <f>COUNTIF(VanillaSwap!D3:D22,"PASS")</f>
         <v>20</v>
       </c>
-      <c r="E35">
-        <f>SUM(C35:D35)</f>
+      <c r="E36">
+        <f>SUM(C36:D36)</f>
         <v>20</v>
       </c>
-      <c r="F35" s="7">
-        <f>D35/E35</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>934</v>
-      </c>
-      <c r="B36">
+      <c r="F36" s="7">
+        <f>D36/E36</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>937</v>
+      </c>
+      <c r="B37">
         <f>COUNTIF(Volatilities!D3:D36,"ERROR")</f>
         <v>7</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <f>COUNTIF(Volatilities!D3:D36,"FAIL")</f>
-        <v>1</v>
-      </c>
-      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="D37">
         <f>COUNTIF(Volatilities!D3:D36,"PASS")</f>
-        <v>26</v>
-      </c>
-      <c r="E36">
-        <f>SUM(C36:D36)</f>
+        <v>22</v>
+      </c>
+      <c r="E37">
+        <f>SUM(C37:D37)</f>
         <v>27</v>
       </c>
-      <c r="F36" s="7">
-        <f>D36/E36</f>
-        <v>0.96296296296296291</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="F37" s="7">
+        <f>D37/E37</f>
+        <v>0.81481481481481477</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="1">
-        <f>SUM(B2:B36)</f>
+      <c r="B38" s="1">
+        <f>SUM(B2:B37)</f>
         <v>108</v>
       </c>
-      <c r="C37" s="1">
-        <f>SUM(C2:C36)</f>
-        <v>22</v>
-      </c>
-      <c r="D37" s="1">
-        <f>SUM(D2:D36)</f>
-        <v>565</v>
-      </c>
-      <c r="E37" s="1">
-        <f>SUM(E2:E36)</f>
-        <v>587</v>
-      </c>
-      <c r="F37" s="8">
-        <f>D37/E37</f>
-        <v>0.96252129471890968</v>
+      <c r="C38" s="1">
+        <f>SUM(C2:C37)</f>
+        <v>25</v>
+      </c>
+      <c r="D38" s="1">
+        <f>SUM(D2:D37)</f>
+        <v>564</v>
+      </c>
+      <c r="E38" s="1">
+        <f>SUM(E2:E37)</f>
+        <v>589</v>
+      </c>
+      <c r="F38" s="8">
+        <f>D38/E38</f>
+        <v>0.95755517826825132</v>
       </c>
     </row>
   </sheetData>
@@ -8636,6 +8672,87 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>558</v>
+      </c>
+      <c r="B3">
+        <v>1.5</v>
+      </c>
+      <c r="C3">
+        <v>1.5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>559</v>
+      </c>
+      <c r="B4">
+        <v>1.5</v>
+      </c>
+      <c r="C4">
+        <v>1.5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8678,7 +8795,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="B3">
         <v>0.38292492254802624</v>
@@ -8695,7 +8812,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B4">
         <v>0.30853753872598688</v>
@@ -8712,7 +8829,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="B5">
         <v>2.5066282746310002</v>
@@ -8729,7 +8846,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -8746,7 +8863,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="B7">
         <v>0.35206532676429952</v>
@@ -8763,7 +8880,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="B8">
         <v>0.3989422804014327</v>
@@ -8780,7 +8897,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="B9">
         <v>2.5066282746309976</v>
@@ -8797,7 +8914,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="B10" t="e">
         <v>#NUM!</v>
@@ -8814,7 +8931,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="B11" t="e">
         <v>#NUM!</v>
@@ -8831,7 +8948,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="B12" t="e">
         <v>#NUM!</v>
@@ -8848,7 +8965,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="B13" t="e">
         <v>#NUM!</v>
@@ -8865,7 +8982,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="B14" t="e">
         <v>#NUM!</v>
@@ -8882,7 +8999,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="B15" t="e">
         <v>#NUM!</v>
@@ -8899,7 +9016,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="B16">
         <v>0.38292492254802624</v>
@@ -8916,7 +9033,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="B17">
         <v>0.69146246127401323</v>
@@ -8933,7 +9050,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="B18">
         <v>0.69146246127401323</v>
@@ -8950,7 +9067,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B19">
         <v>1.8057389857858896</v>
@@ -8967,7 +9084,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="B20">
         <v>1.8057389857858896</v>
@@ -8984,7 +9101,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="B21">
         <v>0.35206532676429947</v>
@@ -9001,7 +9118,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="B22">
         <v>0.35206532676429947</v>
@@ -9018,7 +9135,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="B23">
         <v>-0.17603266338214973</v>
@@ -9035,7 +9152,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="B24">
         <v>-4.8228126954013624E-4</v>
@@ -9052,7 +9169,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="B25">
         <v>0.35206532676429952</v>
@@ -9069,7 +9186,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="B26">
         <v>0.30853753872598699</v>
@@ -9086,7 +9203,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="B27">
         <v>-0.69146246127401323</v>
@@ -9103,7 +9220,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="B28">
         <v>0.30853753872598688</v>
@@ -9120,7 +9237,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="B29">
         <v>0.69146246127401312</v>
@@ -9137,7 +9254,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="B30">
         <v>-0.30853753872598688</v>
@@ -9154,7 +9271,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="B31">
         <v>0.69146246127401312</v>
@@ -9171,7 +9288,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B32">
         <v>-0.30853753872598688</v>
@@ -9188,41 +9305,41 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="B33" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="C33" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="D33" t="s">
         <v>15</v>
       </c>
       <c r="E33" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="B34" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="C34" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="D34" t="s">
         <v>15</v>
       </c>
       <c r="E34" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="B35">
         <v>0.69146246127401323</v>
@@ -9239,7 +9356,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="B36">
         <v>1.8057389857858896</v>
@@ -9256,7 +9373,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="B37">
         <v>0.35206532676429947</v>
@@ -9273,7 +9390,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="B38">
         <v>-0.17603266338214973</v>
@@ -9290,7 +9407,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="B39">
         <v>-4.8228126954013624E-4</v>
@@ -9307,274 +9424,274 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="B40" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="C40" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="D40" t="s">
         <v>15</v>
       </c>
       <c r="E40" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="B41" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="C41" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="D41" t="s">
         <v>15</v>
       </c>
       <c r="E41" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="B42" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="C42" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="D42" t="s">
         <v>15</v>
       </c>
       <c r="E42" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="B43" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="C43" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="D43" t="s">
         <v>15</v>
       </c>
       <c r="E43" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B44" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="C44" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="D44" t="s">
         <v>15</v>
       </c>
       <c r="E44" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="B45" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="C45" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="D45" t="s">
         <v>15</v>
       </c>
       <c r="E45" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="B46" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="C46" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="D46" t="s">
         <v>15</v>
       </c>
       <c r="E46" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="B47" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="C47" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="D47" t="s">
         <v>15</v>
       </c>
       <c r="E47" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="B48" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="C48" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="D48" t="s">
         <v>15</v>
       </c>
       <c r="E48" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="B49" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="C49" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="D49" t="s">
         <v>15</v>
       </c>
       <c r="E49" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="B50" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="C50" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="D50" t="s">
         <v>15</v>
       </c>
       <c r="E50" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="B51" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="C51" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="D51" t="s">
         <v>15</v>
       </c>
       <c r="E51" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="B52" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="C52" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="D52" t="s">
         <v>15</v>
       </c>
       <c r="E52" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="B53" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="C53" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="D53" t="s">
         <v>15</v>
       </c>
       <c r="E53" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="B54" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="C54" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="D54" t="s">
         <v>15</v>
       </c>
       <c r="E54" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="B55" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="C55" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="D55" t="s">
         <v>15</v>
       </c>
       <c r="E55" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
     </row>
   </sheetData>
@@ -9582,7 +9699,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -9626,19 +9743,19 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="B3" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="C3" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
     </row>
   </sheetData>
@@ -9646,7 +9763,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -9690,7 +9807,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="B3">
         <v>123</v>
@@ -9707,7 +9824,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -9724,7 +9841,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -9741,7 +9858,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -9758,7 +9875,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -9775,7 +9892,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B8">
         <v>456</v>
@@ -9792,7 +9909,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -9800,7 +9917,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
@@ -9808,7 +9925,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
@@ -9816,126 +9933,126 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="B12" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="C12" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="B13" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="C13" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="B14" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="C14" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="B15" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="C15" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="B16" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="C16" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="B17" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="C17" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="B18" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="C18" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="B19">
         <v>456</v>
@@ -9952,7 +10069,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="B20">
         <v>789</v>
@@ -9969,7 +10086,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="B21">
         <v>43544</v>
@@ -9986,7 +10103,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="B22">
         <v>123</v>
@@ -10003,24 +10120,24 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B23" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="C23" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="D23" t="s">
         <v>15</v>
       </c>
       <c r="E23" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="B24">
         <v>42644</v>
@@ -10037,19 +10154,19 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="B25" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="C25" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
     </row>
   </sheetData>
@@ -10057,7 +10174,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
@@ -10101,7 +10218,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="B3">
         <v>42648</v>
@@ -10118,7 +10235,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="B4">
         <v>42649</v>
@@ -10135,7 +10252,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="B5">
         <v>42649</v>
@@ -10152,7 +10269,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="B6" s="6">
         <v>42649</v>
@@ -10169,7 +10286,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="C7" t="s">
         <v>107</v>
@@ -10183,7 +10300,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -10200,7 +10317,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="B9" s="6" t="e">
         <v>#NUM!</v>
@@ -10217,7 +10334,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="B10" t="e">
         <v>#NUM!</v>
@@ -10234,75 +10351,75 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="B11" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="C11" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="B12" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="C12" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="B13" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="C13" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="B14" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="C14" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -10319,78 +10436,78 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B16" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="C16" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="B17" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="C17" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="B18" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="C18" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="B19" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
       <c r="C19" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="B20" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="C20" t="e">
         <v>#NAME?</v>
@@ -10404,10 +10521,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="B21" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="C21" t="e">
         <v>#NAME?</v>
@@ -10421,7 +10538,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -10438,75 +10555,75 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="B23" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="C23" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="D23" t="s">
         <v>15</v>
       </c>
       <c r="E23" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
       <c r="B24" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="C24" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="D24" t="s">
         <v>15</v>
       </c>
       <c r="E24" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="B25" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="C25" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
       <c r="B26" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="C26" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="D26" t="s">
         <v>15</v>
       </c>
       <c r="E26" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -10523,24 +10640,24 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="B28" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="C28" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="D28" t="s">
         <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -10557,7 +10674,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="B30" t="s">
         <v>49</v>
@@ -10574,7 +10691,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="B31" t="s">
         <v>147</v>
@@ -10591,7 +10708,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
@@ -10608,7 +10725,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="B33" t="b">
         <v>1</v>
@@ -10625,24 +10742,24 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="B34" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="C34" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="D34" t="s">
         <v>12</v>
       </c>
       <c r="E34" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -10662,7 +10779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
@@ -10706,7 +10823,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -10723,7 +10840,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="B4" s="6">
         <v>25573</v>
@@ -10740,7 +10857,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -10757,7 +10874,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="B6" s="6">
         <v>25570</v>
@@ -10774,7 +10891,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -10791,7 +10908,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
@@ -10808,7 +10925,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>49</v>
@@ -10825,7 +10942,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="B10" s="6">
         <v>25570</v>
@@ -10842,7 +10959,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="B11" s="6">
         <v>25573</v>
@@ -10859,7 +10976,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="B12" t="s">
         <v>231</v>
@@ -10876,7 +10993,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="B13" t="s">
         <v>147</v>
@@ -10893,7 +11010,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="B14" t="s">
         <v>147</v>
@@ -10910,87 +11027,87 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="B15" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
       <c r="C15" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="B16" t="b">
         <v>0</v>
       </c>
       <c r="C16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="B17" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="C17" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="B18" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
       <c r="C18" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="B19" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="C19" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
     </row>
   </sheetData>
@@ -10998,7 +11115,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
@@ -11042,41 +11159,41 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="B3" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="C3" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="B4" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
       <c r="C4" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>743</v>
+        <v>746</v>
       </c>
       <c r="B5">
         <v>2.6897035576518178E-3</v>
@@ -11093,7 +11210,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="B6">
         <v>0.1</v>
@@ -11110,7 +11227,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
       <c r="B7">
         <v>0.05</v>
@@ -11127,7 +11244,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>746</v>
+        <v>749</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -11144,7 +11261,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
       <c r="B9">
         <v>0.01</v>
@@ -11161,24 +11278,24 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
       <c r="B10" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
       <c r="C10" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
       <c r="B11">
         <v>0.1</v>
@@ -11195,7 +11312,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>751</v>
+        <v>754</v>
       </c>
       <c r="B12">
         <v>0.01</v>
@@ -11212,7 +11329,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>752</v>
+        <v>755</v>
       </c>
       <c r="B13">
         <v>0.1</v>
@@ -11229,7 +11346,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="B14">
         <v>0.01</v>
@@ -11246,7 +11363,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>754</v>
+        <v>757</v>
       </c>
       <c r="B15">
         <v>-0.75</v>
@@ -11259,359 +11376,6 @@
       </c>
       <c r="E15">
         <v>-0.75</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>756</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>757</v>
-      </c>
-      <c r="B4">
-        <v>2.7777777777777779E-3</v>
-      </c>
-      <c r="C4">
-        <v>2.7777777777777779E-3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4">
-        <v>2.7777777777777779E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>758</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>759</v>
-      </c>
-      <c r="B6" s="6">
-        <v>42645</v>
-      </c>
-      <c r="C6" s="6">
-        <v>42645</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="6">
-        <v>42645</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>760</v>
-      </c>
-      <c r="B7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C7" t="s">
-        <v>143</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>761</v>
-      </c>
-      <c r="B8" t="s">
-        <v>762</v>
-      </c>
-      <c r="C8" t="s">
-        <v>762</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>763</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>764</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>764</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>765</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>766</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>766</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>767</v>
-      </c>
-      <c r="B11" s="6" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="C11" s="6" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="6" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>768</v>
-      </c>
-      <c r="B12" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="C12" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>769</v>
-      </c>
-      <c r="B13" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="C13" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="D13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>770</v>
-      </c>
-      <c r="B14" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="C14" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="D14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>771</v>
-      </c>
-      <c r="B15" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="C15" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>772</v>
-      </c>
-      <c r="B16" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="C16" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>773</v>
-      </c>
-      <c r="B17" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="C17" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="D17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>774</v>
-      </c>
-      <c r="B18" t="s">
-        <v>775</v>
-      </c>
-      <c r="C18" t="s">
-        <v>775</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>776</v>
-      </c>
-      <c r="B19" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C19" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>777</v>
-      </c>
-      <c r="B20" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="C20" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="D20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" t="e">
-        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>
@@ -11889,6 +11653,359 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>759</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>760</v>
+      </c>
+      <c r="B4">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="C4">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>2.7777777777777779E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>761</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>762</v>
+      </c>
+      <c r="B6" s="6">
+        <v>42645</v>
+      </c>
+      <c r="C6" s="6">
+        <v>42645</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="6">
+        <v>42645</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>763</v>
+      </c>
+      <c r="B7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>764</v>
+      </c>
+      <c r="B8" t="s">
+        <v>765</v>
+      </c>
+      <c r="C8" t="s">
+        <v>765</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>766</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>767</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>767</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>768</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>769</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>769</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>770</v>
+      </c>
+      <c r="B11" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="C11" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="6" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>771</v>
+      </c>
+      <c r="B12" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="C12" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>772</v>
+      </c>
+      <c r="B13" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="C13" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>773</v>
+      </c>
+      <c r="B14" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="C14" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>774</v>
+      </c>
+      <c r="B15" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="C15" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>775</v>
+      </c>
+      <c r="B16" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="C16" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>776</v>
+      </c>
+      <c r="B17" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="C17" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>777</v>
+      </c>
+      <c r="B18" t="s">
+        <v>778</v>
+      </c>
+      <c r="C18" t="s">
+        <v>778</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>779</v>
+      </c>
+      <c r="B19" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C19" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>780</v>
+      </c>
+      <c r="B20" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="C20" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11931,41 +12048,41 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>779</v>
+        <v>782</v>
       </c>
       <c r="B3" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="C3" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>781</v>
+        <v>784</v>
       </c>
       <c r="B4" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c r="C4" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>783</v>
+        <v>786</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -11982,7 +12099,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>784</v>
+        <v>787</v>
       </c>
       <c r="B6">
         <v>-4.9591843073892612</v>
@@ -11999,7 +12116,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>785</v>
+        <v>788</v>
       </c>
       <c r="B7">
         <v>42645</v>
@@ -12016,7 +12133,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>786</v>
+        <v>789</v>
       </c>
       <c r="B8">
         <v>42647</v>
@@ -12033,7 +12150,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>787</v>
+        <v>790</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
@@ -12053,7 +12170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
@@ -12097,7 +12214,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>789</v>
+        <v>792</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -12114,7 +12231,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>790</v>
+        <v>793</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -12131,7 +12248,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
       <c r="B5">
         <v>7.4999999999999997E-2</v>
@@ -12148,7 +12265,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
       <c r="B6">
         <v>8.611111111111111E-2</v>
@@ -12165,24 +12282,24 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
       <c r="B7" t="s">
-        <v>794</v>
+        <v>797</v>
       </c>
       <c r="C7" t="s">
-        <v>794</v>
+        <v>797</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>794</v>
+        <v>797</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="B8" t="s">
         <v>147</v>
@@ -12199,7 +12316,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>796</v>
+        <v>799</v>
       </c>
       <c r="B9" s="3">
         <v>42678</v>
@@ -12216,7 +12333,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>797</v>
+        <v>800</v>
       </c>
       <c r="B10">
         <v>8.3333333333333329E-2</v>
@@ -12233,7 +12350,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>798</v>
+        <v>801</v>
       </c>
       <c r="B11">
         <v>8.3333333333333329E-2</v>
@@ -12250,58 +12367,58 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>799</v>
+        <v>802</v>
       </c>
       <c r="B12" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="C12" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>801</v>
+        <v>804</v>
       </c>
       <c r="B13" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="C13" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>803</v>
+        <v>806</v>
       </c>
       <c r="B14" t="s">
-        <v>804</v>
+        <v>807</v>
       </c>
       <c r="C14" t="s">
-        <v>804</v>
+        <v>807</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>804</v>
+        <v>807</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>805</v>
+        <v>808</v>
       </c>
       <c r="B15" t="e">
         <v>#N/A</v>
@@ -12318,7 +12435,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>806</v>
+        <v>809</v>
       </c>
       <c r="B16" t="e">
         <v>#N/A</v>
@@ -12335,7 +12452,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>807</v>
+        <v>810</v>
       </c>
       <c r="B17" t="e">
         <v>#N/A</v>
@@ -12352,7 +12469,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>808</v>
+        <v>811</v>
       </c>
       <c r="B18" t="e">
         <v>#N/A</v>
@@ -12369,7 +12486,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>809</v>
+        <v>812</v>
       </c>
       <c r="B19" t="e">
         <v>#N/A</v>
@@ -12386,7 +12503,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>810</v>
+        <v>813</v>
       </c>
       <c r="B20" t="e">
         <v>#NUM!</v>
@@ -12403,7 +12520,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>811</v>
+        <v>814</v>
       </c>
       <c r="B21" t="e">
         <v>#N/A</v>
@@ -12420,7 +12537,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>812</v>
+        <v>815</v>
       </c>
       <c r="B22" t="e">
         <v>#N/A</v>
@@ -12437,7 +12554,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="B23" t="e">
         <v>#NUM!</v>
@@ -12454,7 +12571,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>814</v>
+        <v>817</v>
       </c>
       <c r="B24" t="e">
         <v>#N/A</v>
@@ -12471,7 +12588,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>815</v>
+        <v>818</v>
       </c>
       <c r="B25" t="e">
         <v>#N/A</v>
@@ -12488,7 +12605,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>816</v>
+        <v>819</v>
       </c>
       <c r="B26" t="e">
         <v>#N/A</v>
@@ -12505,7 +12622,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>817</v>
+        <v>820</v>
       </c>
       <c r="B27" t="e">
         <v>#N/A</v>
@@ -12522,7 +12639,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>818</v>
+        <v>821</v>
       </c>
       <c r="B28" t="e">
         <v>#VALUE!</v>
@@ -12539,7 +12656,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>819</v>
+        <v>822</v>
       </c>
       <c r="B29" t="e">
         <v>#VALUE!</v>
@@ -12559,7 +12676,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -12603,24 +12720,24 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>821</v>
+        <v>824</v>
       </c>
       <c r="B3" t="s">
-        <v>822</v>
+        <v>825</v>
       </c>
       <c r="C3" t="s">
-        <v>822</v>
+        <v>825</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>822</v>
+        <v>825</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>823</v>
+        <v>826</v>
       </c>
       <c r="B4">
         <v>42738</v>
@@ -12637,7 +12754,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="B5">
         <v>42736</v>
@@ -12654,7 +12771,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -12671,7 +12788,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>826</v>
+        <v>829</v>
       </c>
       <c r="B7" t="s">
         <v>49</v>
@@ -12688,7 +12805,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>827</v>
+        <v>830</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -12705,7 +12822,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>828</v>
+        <v>831</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -12722,7 +12839,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>829</v>
+        <v>832</v>
       </c>
       <c r="B10">
         <v>-180</v>
@@ -12739,7 +12856,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>830</v>
+        <v>833</v>
       </c>
       <c r="B11">
         <v>-180</v>
@@ -12756,7 +12873,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>831</v>
+        <v>834</v>
       </c>
       <c r="B12">
         <v>-252.99872090438052</v>
@@ -12773,143 +12890,143 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>832</v>
+        <v>835</v>
       </c>
       <c r="B13" t="s">
-        <v>833</v>
+        <v>836</v>
       </c>
       <c r="C13" t="s">
-        <v>833</v>
+        <v>836</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>833</v>
+        <v>836</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>834</v>
+        <v>837</v>
       </c>
       <c r="B14" t="s">
-        <v>835</v>
+        <v>838</v>
       </c>
       <c r="C14" t="s">
-        <v>835</v>
+        <v>838</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>835</v>
+        <v>838</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>836</v>
+        <v>839</v>
       </c>
       <c r="B15" t="s">
-        <v>837</v>
+        <v>840</v>
       </c>
       <c r="C15" t="s">
-        <v>837</v>
+        <v>840</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>837</v>
+        <v>840</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>838</v>
+        <v>841</v>
       </c>
       <c r="B16" t="s">
-        <v>839</v>
+        <v>842</v>
       </c>
       <c r="C16" t="s">
-        <v>839</v>
+        <v>842</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>839</v>
+        <v>842</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>840</v>
+        <v>843</v>
       </c>
       <c r="B17" t="s">
-        <v>841</v>
+        <v>844</v>
       </c>
       <c r="C17" t="s">
-        <v>841</v>
+        <v>844</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>841</v>
+        <v>844</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>842</v>
+        <v>845</v>
       </c>
       <c r="B18" t="s">
-        <v>843</v>
+        <v>846</v>
       </c>
       <c r="C18" t="s">
-        <v>843</v>
+        <v>846</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>843</v>
+        <v>846</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>844</v>
+        <v>847</v>
       </c>
       <c r="B19" t="s">
-        <v>845</v>
+        <v>848</v>
       </c>
       <c r="C19" t="s">
-        <v>845</v>
+        <v>848</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>845</v>
+        <v>848</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>846</v>
+        <v>849</v>
       </c>
       <c r="B20" t="s">
-        <v>847</v>
+        <v>850</v>
       </c>
       <c r="C20" t="s">
-        <v>847</v>
+        <v>850</v>
       </c>
       <c r="D20" t="s">
         <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>847</v>
+        <v>850</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>848</v>
+        <v>851</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -12926,7 +13043,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>849</v>
+        <v>852</v>
       </c>
       <c r="B22">
         <v>42736</v>
@@ -12943,7 +13060,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>850</v>
+        <v>853</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -12960,7 +13077,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>851</v>
+        <v>854</v>
       </c>
       <c r="B24">
         <v>8.3333333333333332E-3</v>
@@ -12977,7 +13094,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>852</v>
+        <v>855</v>
       </c>
       <c r="B25">
         <v>42739</v>
@@ -12997,7 +13114,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -13041,24 +13158,24 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>854</v>
+        <v>857</v>
       </c>
       <c r="B3" t="s">
-        <v>855</v>
+        <v>858</v>
       </c>
       <c r="C3" t="s">
-        <v>855</v>
+        <v>858</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>855</v>
+        <v>858</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c r="B4">
         <v>25569</v>
@@ -13075,7 +13192,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>857</v>
+        <v>860</v>
       </c>
       <c r="B5">
         <v>25571</v>
@@ -13092,7 +13209,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>858</v>
+        <v>861</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -13109,7 +13226,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>859</v>
+        <v>862</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
@@ -13126,7 +13243,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>860</v>
+        <v>863</v>
       </c>
       <c r="B8">
         <v>25569</v>
@@ -13143,7 +13260,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>861</v>
+        <v>864</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -13160,7 +13277,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>862</v>
+        <v>865</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -13177,7 +13294,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>863</v>
+        <v>866</v>
       </c>
       <c r="B11" t="e">
         <v>#NUM!</v>
@@ -13197,7 +13314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -13241,19 +13358,19 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="B3" t="s">
-        <v>866</v>
+        <v>869</v>
       </c>
       <c r="C3" t="s">
-        <v>867</v>
+        <v>870</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>867</v>
+        <v>870</v>
       </c>
     </row>
   </sheetData>
@@ -13261,7 +13378,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
@@ -13305,92 +13422,92 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>869</v>
+        <v>872</v>
       </c>
       <c r="B3" t="s">
-        <v>870</v>
+        <v>873</v>
       </c>
       <c r="C3" t="s">
-        <v>870</v>
+        <v>873</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>870</v>
+        <v>873</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>871</v>
+        <v>874</v>
       </c>
       <c r="B4" t="s">
-        <v>872</v>
+        <v>875</v>
       </c>
       <c r="C4" t="s">
-        <v>872</v>
+        <v>875</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>872</v>
+        <v>875</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>873</v>
+        <v>876</v>
       </c>
       <c r="B5" t="s">
-        <v>874</v>
+        <v>877</v>
       </c>
       <c r="C5" t="s">
-        <v>874</v>
+        <v>877</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>874</v>
+        <v>877</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>875</v>
+        <v>878</v>
       </c>
       <c r="B6" t="s">
-        <v>876</v>
+        <v>879</v>
       </c>
       <c r="C6" t="s">
-        <v>876</v>
+        <v>879</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>876</v>
+        <v>879</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>877</v>
+        <v>880</v>
       </c>
       <c r="B7" t="s">
-        <v>878</v>
+        <v>881</v>
       </c>
       <c r="C7" t="s">
-        <v>878</v>
+        <v>881</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>878</v>
+        <v>881</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>879</v>
+        <v>882</v>
       </c>
       <c r="B8">
         <v>-0.67739587129550227</v>
@@ -13407,7 +13524,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>880</v>
+        <v>883</v>
       </c>
       <c r="B9">
         <v>-33869.793564775115</v>
@@ -13424,7 +13541,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>881</v>
+        <v>884</v>
       </c>
       <c r="B10">
         <v>142.62616569880501</v>
@@ -13441,7 +13558,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>882</v>
+        <v>885</v>
       </c>
       <c r="B11">
         <v>4.477796795487806</v>
@@ -13458,7 +13575,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>883</v>
+        <v>886</v>
       </c>
       <c r="B12">
         <v>966143.7578307871</v>
@@ -13475,7 +13592,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>884</v>
+        <v>887</v>
       </c>
       <c r="B13">
         <v>-20.819925665350592</v>
@@ -13492,24 +13609,24 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c r="B14" t="s">
-        <v>886</v>
+        <v>889</v>
       </c>
       <c r="C14" t="s">
-        <v>886</v>
+        <v>889</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>886</v>
+        <v>889</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>887</v>
+        <v>890</v>
       </c>
       <c r="B15">
         <v>1000000</v>
@@ -13526,7 +13643,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>888</v>
+        <v>891</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -13543,24 +13660,24 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>889</v>
+        <v>892</v>
       </c>
       <c r="B17" t="s">
-        <v>890</v>
+        <v>893</v>
       </c>
       <c r="C17" t="s">
-        <v>890</v>
+        <v>893</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>890</v>
+        <v>893</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>891</v>
+        <v>894</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -13577,7 +13694,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>892</v>
+        <v>895</v>
       </c>
       <c r="B19" t="s">
         <v>143</v>
@@ -13594,24 +13711,24 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>893</v>
+        <v>896</v>
       </c>
       <c r="B20" t="s">
-        <v>894</v>
+        <v>897</v>
       </c>
       <c r="C20" t="s">
-        <v>894</v>
+        <v>897</v>
       </c>
       <c r="D20" t="s">
         <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>894</v>
+        <v>897</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>895</v>
+        <v>898</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -13628,7 +13745,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>896</v>
+        <v>899</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
@@ -13648,7 +13765,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
@@ -13692,7 +13809,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="B3">
         <v>23.948673390030997</v>
@@ -13709,24 +13826,24 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>899</v>
+        <v>902</v>
       </c>
       <c r="B4" t="s">
-        <v>894</v>
+        <v>897</v>
       </c>
       <c r="C4" t="s">
-        <v>894</v>
+        <v>897</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>894</v>
+        <v>897</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>900</v>
+        <v>903</v>
       </c>
       <c r="B5">
         <v>42648</v>
@@ -13743,7 +13860,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="B6">
         <v>-1.7976931348623157E+308</v>
@@ -13760,7 +13877,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>902</v>
+        <v>905</v>
       </c>
       <c r="B7">
         <v>1.7976931348623157E+308</v>
@@ -13777,7 +13894,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="B8" t="e">
         <v>#NUM!</v>
@@ -13794,7 +13911,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>904</v>
+        <v>907</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -13811,7 +13928,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>905</v>
+        <v>908</v>
       </c>
       <c r="B10">
         <v>3.3161907871456142</v>
@@ -13828,7 +13945,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>906</v>
+        <v>909</v>
       </c>
       <c r="B11" t="e">
         <v>#NUM!</v>
@@ -13845,7 +13962,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>907</v>
+        <v>910</v>
       </c>
       <c r="B12">
         <v>2.7777777777777779E-3</v>
@@ -13862,7 +13979,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>908</v>
+        <v>911</v>
       </c>
       <c r="B13">
         <v>0.10997121336749448</v>
@@ -13879,7 +13996,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>909</v>
+        <v>912</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -13896,7 +14013,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>910</v>
+        <v>913</v>
       </c>
       <c r="B15">
         <v>2.7777777777777779E-3</v>
@@ -13913,7 +14030,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>911</v>
+        <v>914</v>
       </c>
       <c r="B16">
         <v>1.0000000000000011</v>
@@ -13930,7 +14047,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>912</v>
+        <v>915</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -13947,24 +14064,24 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>913</v>
+        <v>916</v>
       </c>
       <c r="B18" t="s">
-        <v>914</v>
+        <v>917</v>
       </c>
       <c r="C18" t="s">
-        <v>914</v>
+        <v>917</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>914</v>
+        <v>917</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>915</v>
+        <v>918</v>
       </c>
       <c r="B19" t="e">
         <v>#VALUE!</v>
@@ -13981,7 +14098,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>916</v>
+        <v>919</v>
       </c>
       <c r="B20" t="s">
         <v>231</v>
@@ -13998,7 +14115,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>917</v>
+        <v>920</v>
       </c>
       <c r="B21" t="s">
         <v>231</v>
@@ -14015,7 +14132,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>918</v>
+        <v>921</v>
       </c>
       <c r="B22">
         <v>42648</v>
@@ -14032,7 +14149,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>919</v>
+        <v>922</v>
       </c>
       <c r="B23">
         <v>2.7777777777777779E-3</v>
@@ -14049,75 +14166,75 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>920</v>
+        <v>923</v>
       </c>
       <c r="B24">
         <v>0.16276901888733139</v>
       </c>
       <c r="C24">
-        <v>0.16276901888733139</v>
+        <v>0.16276967485704383</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E24">
-        <v>0.16276901888733139</v>
+        <v>0.16276967485704383</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>921</v>
+        <v>924</v>
       </c>
       <c r="B25">
         <v>0.20553128316863267</v>
       </c>
       <c r="C25">
-        <v>0.20553128316863267</v>
+        <v>0.20543416674806414</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E25">
-        <v>0.20553128316863267</v>
+        <v>0.20543416674806414</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>922</v>
+        <v>925</v>
       </c>
       <c r="B26">
         <v>-5.6930143586703347E-4</v>
       </c>
       <c r="C26">
-        <v>-5.6930143586703347E-4</v>
+        <v>-1.1138084851759278E-3</v>
       </c>
       <c r="D26" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E26">
-        <v>-5.6930143586703347E-4</v>
+        <v>-1.1138084851759278E-3</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>923</v>
+        <v>926</v>
       </c>
       <c r="B27">
         <v>816.38970366714</v>
       </c>
       <c r="C27">
-        <v>816.38970366714</v>
+        <v>816.38481984485099</v>
       </c>
       <c r="D27" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E27">
-        <v>816.38970366714</v>
+        <v>816.38481984485099</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>924</v>
+        <v>927</v>
       </c>
       <c r="B28">
         <v>55.846414299893993</v>
@@ -14134,41 +14251,41 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>925</v>
+        <v>928</v>
       </c>
       <c r="B29">
         <v>5.6930143586703347E-4</v>
       </c>
       <c r="C29">
-        <v>1.1139404844395559E-3</v>
+        <v>5.6930143586703347E-4</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E29">
-        <v>1.1139404844395559E-3</v>
+        <v>5.6930143586703347E-4</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B30">
         <v>0.85719125008922603</v>
       </c>
       <c r="C30">
-        <v>0.85719125008922603</v>
+        <v>0.85716351011528225</v>
       </c>
       <c r="D30" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E30">
-        <v>0.85719125008922603</v>
+        <v>0.85716351011528225</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>927</v>
+        <v>930</v>
       </c>
       <c r="B31">
         <v>1.0563094653822682</v>
@@ -14185,24 +14302,24 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>928</v>
+        <v>931</v>
       </c>
       <c r="B32" t="s">
-        <v>929</v>
+        <v>932</v>
       </c>
       <c r="C32" t="s">
-        <v>929</v>
+        <v>932</v>
       </c>
       <c r="D32" t="s">
         <v>15</v>
       </c>
       <c r="E32" t="s">
-        <v>929</v>
+        <v>932</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>930</v>
+        <v>933</v>
       </c>
       <c r="B33" t="e">
         <v>#NUM!</v>
@@ -14219,7 +14336,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>931</v>
+        <v>934</v>
       </c>
       <c r="B34" t="e">
         <v>#VALUE!</v>
@@ -14236,7 +14353,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>932</v>
+        <v>935</v>
       </c>
       <c r="B35" t="e">
         <v>#VALUE!</v>
@@ -14253,7 +14370,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>933</v>
+        <v>936</v>
       </c>
       <c r="B36" t="e">
         <v>#VALUE!</v>

</xml_diff>